<commit_message>
add bonus mision 3
</commit_message>
<xml_diff>
--- a/Orkos/1. Datos.xlsx
+++ b/Orkos/1. Datos.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Kapitan Bluddflagg</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Martillo enorme</t>
+  </si>
+  <si>
+    <t>Armadura</t>
   </si>
 </sst>
 </file>
@@ -782,10 +785,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,10 +830,110 @@
         <v>15</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
correction Nº2 about skills order
</commit_message>
<xml_diff>
--- a/Orkos/1. Datos.xlsx
+++ b/Orkos/1. Datos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Habilidades" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Kapitan Bluddflagg</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Armadura</t>
+  </si>
+  <si>
+    <t>Habilidades cuantificadas</t>
+  </si>
+  <si>
+    <t>Orden de habilidades</t>
   </si>
 </sst>
 </file>
@@ -133,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -141,12 +147,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -176,6 +197,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -457,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD15" sqref="AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,149 +499,149 @@
     <col min="10" max="16384" width="5.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2">
-        <f>SUM(A2:E2)</f>
-        <v>7.5</v>
-      </c>
+      <c r="T1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="C3" s="3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
-        <f t="shared" ref="F3:F4" si="0">SUM(A3:E3)</f>
-        <v>6.5</v>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="T3" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="3">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F4" s="2">
+        <f>SUM(A4:E4)</f>
+        <v>7.5</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="8"/>
+      <c r="T4" s="12">
+        <v>2</v>
+      </c>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" ref="F5:F6" si="0">SUM(A5:E5)</f>
+        <v>6.5</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="T5" s="12">
+        <v>1</v>
+      </c>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="F7" s="2">
-        <f>SUM(A7:E7)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="B8" s="8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" ref="F8:F9" si="1">SUM(A8:E8)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>0.5</v>
       </c>
@@ -624,162 +651,267 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="5">
-        <v>1.5</v>
+      <c r="D9" s="7">
+        <v>2</v>
       </c>
       <c r="E9" s="3">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F9" s="2">
+        <f>SUM(A9:E9)</f>
+        <v>6</v>
+      </c>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" ref="F10:F11" si="1">SUM(A10:E10)</f>
+        <v>4</v>
+      </c>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="T11" s="12">
+        <v>1</v>
+      </c>
+      <c r="U11" s="12">
+        <v>2</v>
+      </c>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>1</v>
-      </c>
-      <c r="B12" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="F12" s="2">
-        <f>SUM(A12:E12)</f>
+      <c r="F13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F14" s="2">
+        <f>SUM(A14:E14)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1</v>
-      </c>
-      <c r="D13" s="7">
-        <v>2</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2">
-        <f t="shared" ref="F13:F14" si="2">SUM(A13:E13)</f>
+      <c r="T14" s="12">
+        <v>2</v>
+      </c>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" ref="F15:F16" si="2">SUM(A15:E15)</f>
         <v>6.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>1</v>
-      </c>
-      <c r="B14" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1</v>
-      </c>
-      <c r="D14" s="3">
-        <v>1</v>
-      </c>
-      <c r="E14" s="3">
+      <c r="T15" s="12">
+        <v>1</v>
+      </c>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
         <v>0.5</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F16" s="2">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>1.5</v>
-      </c>
-      <c r="B17" s="8">
-        <v>1.5</v>
-      </c>
-      <c r="C17" s="8">
-        <v>1.5</v>
-      </c>
-      <c r="D17" s="8">
-        <v>1</v>
-      </c>
-      <c r="E17" s="8">
-        <v>1.5</v>
-      </c>
-      <c r="F17" s="2">
-        <f>SUM(A17:E17)</f>
+      <c r="F18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="C19" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D19" s="8">
+        <v>1</v>
+      </c>
+      <c r="E19" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="F19" s="2">
+        <f>SUM(A19:E19)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>1.5</v>
-      </c>
-      <c r="B18" s="8">
-        <v>1</v>
-      </c>
-      <c r="C18" s="8">
-        <v>1</v>
-      </c>
-      <c r="D18" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="E18" s="8">
-        <v>1.5</v>
-      </c>
-      <c r="F18" s="2">
-        <f t="shared" ref="F18:F19" si="3">SUM(A18:E18)</f>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="12"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="B20" s="8">
+        <v>1</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="E20" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" ref="F20:F21" si="3">SUM(A20:E20)</f>
         <v>6.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <v>1</v>
-      </c>
-      <c r="B19" s="8">
-        <v>1</v>
-      </c>
-      <c r="C19" s="8">
-        <v>1</v>
-      </c>
-      <c r="D19" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="E19" s="8">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2">
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="12"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>1</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1</v>
+      </c>
+      <c r="C21" s="8">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="E21" s="8">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
         <f t="shared" si="3"/>
         <v>5.5</v>
       </c>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="12"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="T1:X1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -787,7 +919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
actualizacion de datos 2
</commit_message>
<xml_diff>
--- a/Orkos/1. Datos.xlsx
+++ b/Orkos/1. Datos.xlsx
@@ -487,7 +487,7 @@
   <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,12 +847,8 @@
         <f>SUM(A19:E19)</f>
         <v>7</v>
       </c>
-      <c r="T19" s="11">
-        <v>1</v>
-      </c>
-      <c r="U19" s="11">
-        <v>2</v>
-      </c>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
       <c r="V19" s="11"/>
       <c r="W19" s="11"/>
       <c r="X19" s="11"/>
@@ -877,8 +873,12 @@
         <f t="shared" ref="F20:F21" si="3">SUM(A20:E20)</f>
         <v>6.5</v>
       </c>
-      <c r="T20" s="11"/>
-      <c r="U20" s="11"/>
+      <c r="T20" s="11">
+        <v>1</v>
+      </c>
+      <c r="U20" s="11">
+        <v>2</v>
+      </c>
       <c r="V20" s="11"/>
       <c r="W20" s="11"/>
       <c r="X20" s="11"/>

</xml_diff>